<commit_message>
plan for annotated properties i.e. building shapes out of multiple columns
</commit_message>
<xml_diff>
--- a/LAM-mapping-input.xlsx
+++ b/LAM-mapping-input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27792" windowHeight="13176" tabRatio="416" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27792" windowHeight="13176" tabRatio="416" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="description" sheetId="3" r:id="rId1"/>
@@ -3077,7 +3077,7 @@
   <dimension ref="A1:M83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5752,8 +5752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9546,8 +9546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11331,7 +11331,7 @@
   <dimension ref="A1:W83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="W1" sqref="W1:W1048576"/>
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>